<commit_message>
feat the Series product
1、增加了捆绑的一系列产品
</commit_message>
<xml_diff>
--- a/documents/智慧农业项目开支.xlsx
+++ b/documents/智慧农业项目开支.xlsx
@@ -8,18 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="总表" sheetId="1" r:id="rId1"/>
-    <sheet name="4.7" sheetId="4" r:id="rId2"/>
-    <sheet name="3.20" sheetId="3" r:id="rId3"/>
-    <sheet name="12.28" sheetId="2" r:id="rId4"/>
-    <sheet name="陈嘉彬" sheetId="5" r:id="rId5"/>
-    <sheet name="王开" sheetId="6" r:id="rId6"/>
+    <sheet name="4.22" sheetId="7" r:id="rId2"/>
+    <sheet name="4.7" sheetId="4" r:id="rId3"/>
+    <sheet name="3.20" sheetId="3" r:id="rId4"/>
+    <sheet name="12.28" sheetId="2" r:id="rId5"/>
+    <sheet name="陈嘉彬" sheetId="5" r:id="rId6"/>
+    <sheet name="王开" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -393,6 +394,38 @@
   </si>
   <si>
     <t>黄老师报账</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优信电子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贴片C8T6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贴片2596</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铜柱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转接板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继电器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -766,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1087,6 +1120,20 @@
         <v>218.55</v>
       </c>
     </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
+        <v>4.22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1">
+        <v>35.06</v>
+      </c>
+      <c r="D23" s="1">
+        <v>183.49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,6 +1142,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>B3*C3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D8" si="0">B4*C4</f>
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.19</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>11.899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D9" s="1">
+        <f>SUM(D3:D8)</f>
+        <v>35.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D170"/>
   <sheetViews>
@@ -1638,12 +1843,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2241,7 +2446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2442,12 +2647,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2460,6 +2665,17 @@
         <v>62.85</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B2" s="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B4">
+        <f>SUM(B1:B3)</f>
+        <v>267.85000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2467,7 +2683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>